<commit_message>
Fixed bug with Treasury yield naming (v0.20)
</commit_message>
<xml_diff>
--- a/model-inputs/external-forecasts-manual.xlsx
+++ b/model-inputs/external-forecasts-manual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28AB457F-882B-4256-A66D-F798C204453B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0264566C-1036-4C2B-BA5A-976024A3ECB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7EA91EED-77CB-43E4-BA35-3D98E29C29D5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{7EA91EED-77CB-43E4-BA35-3D98E29C29D5}"/>
   </bookViews>
   <sheets>
     <sheet name="wsj_2021-04-11" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="136">
   <si>
     <t>tyield_10y</t>
   </si>
@@ -444,6 +444,9 @@
   <si>
     <t xml:space="preserve">Grant Thornton </t>
   </si>
+  <si>
+    <t>t10y</t>
+  </si>
 </sst>
 </file>
 
@@ -817,30 +820,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5721CF55-ED0C-43FA-89EE-4708DA134218}">
   <dimension ref="A1:AE80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="AG1" sqref="AG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="E1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="G1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="H1" t="s">
         <v>9</v>
@@ -7182,26 +7185,26 @@
   <dimension ref="A1:AA80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A79"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="E1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="G1" t="s">
         <v>9</v>
@@ -12361,7 +12364,7 @@
   <dimension ref="A1:AH77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="B1" sqref="B1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12371,25 +12374,25 @@
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="E1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="G1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="H1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="I1" t="s">
         <v>9</v>
@@ -18874,8 +18877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1EC6099-6558-47E9-8D3F-494B0DCD210D}">
   <dimension ref="A1:AD76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18887,22 +18890,22 @@
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added initial test code for WFC import (Camelot) & TD import (v0.20)
</commit_message>
<xml_diff>
--- a/model-inputs/external-forecasts-manual.xlsx
+++ b/model-inputs/external-forecasts-manual.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0264566C-1036-4C2B-BA5A-976024A3ECB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3E2F3F-BEEC-4820-959D-690879BB2218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{7EA91EED-77CB-43E4-BA35-3D98E29C29D5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{7EA91EED-77CB-43E4-BA35-3D98E29C29D5}"/>
   </bookViews>
   <sheets>
     <sheet name="wsj_2021-04-11" sheetId="6" r:id="rId1"/>
@@ -18877,8 +18877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1EC6099-6558-47E9-8D3F-494B0DCD210D}">
   <dimension ref="A1:AD76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24779,8 +24779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94FA31AD-7358-41CC-8CFF-326801F7042B}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>